<commit_message>
Added manual trumpf tests
</commit_message>
<xml_diff>
--- a/elbotto/bots/training/manual_test_data/trumpf_results/results_trumpf_list.xlsx
+++ b/elbotto/bots/training/manual_test_data/trumpf_results/results_trumpf_list.xlsx
@@ -524,25 +524,25 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.3410981297492981</v>
+        <v>0.3410980105400085</v>
       </c>
       <c r="L2" t="n">
-        <v>0.04955912753939629</v>
+        <v>0.04955914244055748</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0001130052187363617</v>
+        <v>0.0001130051168729551</v>
       </c>
       <c r="N2" t="n">
-        <v>0.001121656969189644</v>
+        <v>0.001121657551266253</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0006293602637015283</v>
+        <v>0.0006293603219091892</v>
       </c>
       <c r="P2" t="n">
-        <v>0.05612512305378914</v>
+        <v>0.05612513050436974</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.5513536334037781</v>
+        <v>0.5513536930084229</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -583,19 +583,19 @@
         <v>0.1199241951107979</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0001091991143766791</v>
+        <v>0.0001091990125132725</v>
       </c>
       <c r="N3" t="n">
-        <v>0.001672260113991797</v>
+        <v>0.001672260812483728</v>
       </c>
       <c r="O3" t="n">
-        <v>0.00136331922840327</v>
+        <v>0.001363319926895201</v>
       </c>
       <c r="P3" t="n">
-        <v>0.06736108660697937</v>
+        <v>0.06736111640930176</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.006475819274783134</v>
+        <v>0.006475815549492836</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -636,19 +636,19 @@
         <v>0.1199241951107979</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0001091991143766791</v>
+        <v>0.0001091990125132725</v>
       </c>
       <c r="N4" t="n">
-        <v>0.001672260113991797</v>
+        <v>0.001672260812483728</v>
       </c>
       <c r="O4" t="n">
-        <v>0.00136331922840327</v>
+        <v>0.001363319926895201</v>
       </c>
       <c r="P4" t="n">
-        <v>0.06736108660697937</v>
+        <v>0.06736111640930176</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.006475819274783134</v>
+        <v>0.006475815549492836</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -683,25 +683,25 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.448344349861145</v>
+        <v>0.4483442306518555</v>
       </c>
       <c r="L5" t="n">
-        <v>0.04407953098416328</v>
+        <v>0.04407955333590508</v>
       </c>
       <c r="M5" t="n">
-        <v>9.583415521774441e-05</v>
+        <v>9.583416976965964e-05</v>
       </c>
       <c r="N5" t="n">
-        <v>0.00166768510825932</v>
+        <v>0.001667686155997217</v>
       </c>
       <c r="O5" t="n">
-        <v>0.001292201341129839</v>
+        <v>0.001292201573960483</v>
       </c>
       <c r="P5" t="n">
-        <v>0.03173016384243965</v>
+        <v>0.03173017129302025</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.4727902710437775</v>
+        <v>0.4727903604507446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>